<commit_message>
Fix: Wrapped View Results button in layout with stretch for perfect vertical centering
</commit_message>
<xml_diff>
--- a/violations_dashboard.xlsx
+++ b/violations_dashboard.xlsx
@@ -250,7 +250,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'dashboard'!B19</f>
+              <f>'dashboard'!B10</f>
             </strRef>
           </tx>
           <spPr>
@@ -260,12 +260,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'dashboard'!$A$20:$A$29</f>
+              <f>'dashboard'!$A$11:$A$20</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'dashboard'!$B$20:$B$28</f>
+              <f>'dashboard'!$B$11:$B$19</f>
             </numRef>
           </val>
         </ser>
@@ -332,7 +332,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'dashboard'!B34</f>
+              <f>'dashboard'!B18</f>
             </strRef>
           </tx>
           <spPr>
@@ -342,12 +342,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'dashboard'!$A$35:$A$34</f>
+              <f>'dashboard'!$A$19:$A$18</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'dashboard'!$C$34:$B$34</f>
+              <f>'dashboard'!$C$18:$B$18</f>
             </numRef>
           </val>
         </ser>
@@ -413,7 +413,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'dashboard'!B40</f>
+              <f>'dashboard'!B24</f>
             </strRef>
           </tx>
           <spPr>
@@ -431,12 +431,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'dashboard'!$A$41:$A$43</f>
+              <f>'dashboard'!$A$25:$A$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'dashboard'!$B$41:$B$43</f>
+              <f>'dashboard'!$C$24:$B$24</f>
             </numRef>
           </val>
         </ser>
@@ -857,7 +857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -871,12 +871,12 @@
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="26" customWidth="1" min="7" max="7"/>
     <col width="73" customWidth="1" min="8" max="8"/>
     <col width="11" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="24" customWidth="1" min="11" max="11"/>
+    <col width="23" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1104,633 +1104,6 @@
       <c r="K4" t="inlineStr">
         <is>
           <t>116-50 146 STREET</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>08902</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>00063</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-03-05</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>88-15</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>76 STREET</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>88-15 76 STREET</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>03408</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>00048</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-02-28</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>WOODWARD AVENUE</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>614 WOODWARD AVENUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>03552</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>00077</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-02-27</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1659</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>STEPHEN STREET</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>1659 STEPHEN STREET</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>11840</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>00040</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2025-02-27</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>117-18</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>150 AVENUE</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>117-18 150 AVENUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>07405</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>00546</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2025-02-24</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>4433</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>BEDFORD AVENUE</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>4433 BEDFORD AVENUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>15725</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>00048</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2025-02-21</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>11-10</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>WATERVIEW STREET</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>11-10 WATERVIEW STREET</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>14063</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>00018</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2025-02-10</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>162-28</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>90 STREET</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>162-28 90 STREET</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>03671</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>00038</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2025-02-08</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2683</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>ATLANTIC AVENUE</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>2683 ATLANTIC AVENUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>13567</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>00084</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2025-02-04</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>243-58</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>MAYDA ROAD</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>243-58 MAYDA ROAD</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>06120</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>00043</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2025-01-28</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>135</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>96 STREET</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>135 96 STREET</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>07788</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>00002</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2025-01-18</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>4019</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>AVENUE K</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>V-DOB VIOLATION - ACTIVE</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Warm</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>4019 AVENUE K</t>
         </is>
       </c>
     </row>
@@ -1745,7 +1118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1785,17 +1158,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>76 STREET</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>WOODWARD AVENUE</t>
+          <t>116-52 146 STREET</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1805,7 +1180,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STEPHEN STREET</t>
+          <t>116-52 REA 146 STREET</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1815,7 +1190,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>150 AVENUE</t>
+          <t>116-50 146 STREET</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1825,236 +1200,44 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BEDFORD AVENUE</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WATERVIEW STREET</t>
+          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>90 STREET</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
+          <t>Month</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ATLANTIC AVENUE</t>
+          <t>2025-04</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MAYDA ROAD</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>116-52 146 STREET</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>116-52 REA 146 STREET</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>116-50 146 STREET</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>88-15 76 STREET</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>614 WOODWARD AVENUE</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1659 STEPHEN STREET</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>117-18 150 AVENUE</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>4433 BEDFORD AVENUE</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>11-10 WATERVIEW STREET</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>162-28 90 STREET</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>UB-UNSAFE BUILDINGS                                                NONE</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Month</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2025-01</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2025-02</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2025-03</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2025-04</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>